<commit_message>
updated_motifs, 32 plots, mean,max,sum correlation tables
</commit_message>
<xml_diff>
--- a/results/metric_df/ABA_metrics.xlsx
+++ b/results/metric_df/ABA_metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,35 +451,45 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>sum_SASA</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>max_SASA</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>flexibility</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Q</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>theta</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>conformation</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>monosaccharides</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>motifs</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>class</t>
         </is>
@@ -488,166 +498,190 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Fuc(a1-2)Gal(b1-3)GlcNAc(b1-3)[Gal(b1-4)GlcNAc(b1-6)]Gal(b1-4)Glc</t>
+          <t>Fuc(a1-3)[Gal(b1-4)]GlcNAc(b1-2)Man(a1-3)[Fuc(a1-3)[Gal(b1-4)]GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.2577205892445011</v>
+        <v>-0.17559545510933</v>
       </c>
       <c r="C2" t="n">
-        <v>2.488746614678542</v>
+        <v>1.587431760889491</v>
       </c>
       <c r="D2" t="n">
-        <v>13.45695</v>
+        <v>7.937158804447455</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4555</v>
+        <v>1.839230848038921</v>
       </c>
       <c r="F2" t="n">
-        <v>3.73</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-6)']</t>
-        </is>
+        <v>21.81029602960296</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.4232</v>
+      </c>
+      <c r="H2" t="n">
+        <v>6.074</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>lipid/free</t>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Fuc(a1-3)[Gal(b1-4)]GlcNAc</t>
+          <t>Fuc(a1-3)[Gal(b1-4)]GlcNAc(b1-2)Man(a1-3)[Fuc(a1-3)[Gal(b1-4)]GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)[Fuc(a1-6)]GlcNAc</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.2273740767837458</v>
+        <v>-0.2335906390934098</v>
       </c>
       <c r="C3" t="n">
-        <v>2.315462523559917</v>
+        <v>1.606359251840022</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7807833333333334</v>
+        <v>8.03179625920011</v>
       </c>
       <c r="E3" t="n">
-        <v>0.419</v>
+        <v>1.950594211024468</v>
       </c>
       <c r="F3" t="n">
-        <v>7.37</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-1)']</t>
-        </is>
+        <v>18.84326099276594</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.4214000000000001</v>
+      </c>
+      <c r="H3" t="n">
+        <v>4.428</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Fuc(a1-3)[Gal(b1-4)]GlcNAc(b1-2)Man</t>
+          <t>Gal(b1-4)GlcNAc(b1-2)Man(a1-3)[Gal(b1-4)GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.1612855142554764</v>
+        <v>-0.3737560561723356</v>
       </c>
       <c r="C4" t="n">
-        <v>2.095696026530681</v>
+        <v>1.64851644134979</v>
       </c>
       <c r="D4" t="n">
-        <v>0.35245</v>
+        <v>8.242582206748951</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4615</v>
+        <v>2.173258875011851</v>
       </c>
       <c r="F4" t="n">
-        <v>8.545</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-2)']</t>
-        </is>
+        <v>18.37640666666667</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.4354</v>
+      </c>
+      <c r="H4" t="n">
+        <v>10.302</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Fuc(a1-3)[Gal(b1-4)]GlcNAc(b1-2)Man(a1-3)[Fuc(a1-3)[Gal(b1-4)]GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
+          <t>Gal(b1-4)GlcNAc(b1-2)Man(a1-3)[Gal(b1-4)GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)[Fuc(a1-6)]GlcNAc</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.17559545510933</v>
+        <v>-0.3559655680542978</v>
       </c>
       <c r="C5" t="n">
-        <v>1.839862977009192</v>
+        <v>1.80567444172721</v>
       </c>
       <c r="D5" t="n">
-        <v>38.81119986998699</v>
+        <v>9.02837220863605</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4305</v>
+        <v>2.592830414700101</v>
       </c>
       <c r="F5" t="n">
-        <v>9.94</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1', '4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-2)', 'Gal(b1-4)', 'GlcNAc(b1-2)']</t>
-        </is>
+        <v>13.05293</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.4448</v>
+      </c>
+      <c r="H5" t="n">
+        <v>5.36</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -656,40 +690,46 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Fuc(a1-3)[Gal(b1-4)]GlcNAc(b1-2)Man(a1-3)[Fuc(a1-3)[Gal(b1-4)]GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)[Fuc(a1-6)]GlcNAc</t>
+          <t>Gal(b1-4)GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.2335906390934098</v>
+        <v>1.027767814656359</v>
       </c>
       <c r="C6" t="n">
-        <v>1.828098178284811</v>
+        <v>1.934001417720768</v>
       </c>
       <c r="D6" t="n">
-        <v>24.84926826015935</v>
+        <v>9.670007088603839</v>
       </c>
       <c r="E6" t="n">
-        <v>0.45175</v>
+        <v>2.708633284112756</v>
       </c>
       <c r="F6" t="n">
-        <v>3.8825</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1', '4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-2)', 'Gal(b1-4)', 'GlcNAc(b1-2)']</t>
-        </is>
+        <v>10.45456945694569</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.4378</v>
+      </c>
+      <c r="H6" t="n">
+        <v>21.748</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', 'B2,5']</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -698,82 +738,94 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Gal(b1-4)GlcNAc(b1-2)Man</t>
+          <t>Gal(b1-4)GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)[Fuc(a1-6)]GlcNAc</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.1836452615203268</v>
+        <v>1.142698756269506</v>
       </c>
       <c r="C7" t="n">
-        <v>2.597512620302648</v>
+        <v>1.79407827359853</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9847586669904439</v>
+        <v>8.970391367992651</v>
       </c>
       <c r="E7" t="n">
-        <v>0.404</v>
+        <v>2.484382304333421</v>
       </c>
       <c r="F7" t="n">
-        <v>8.209999999999999</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-2)']</t>
-        </is>
+        <v>9.306669333066694</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="H7" t="n">
+        <v>8.704000000000001</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Gal(b1-4)GlcNAc(b1-2)Man(a1-3)[Gal(b1-4)GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
+          <t>Gal(b1-4)GlcNAc(b1-2)Man(a1-6)[GlcNAc(b1-2)Man(a1-3)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.3737560561723356</v>
+        <v>2.392576267477931</v>
       </c>
       <c r="C8" t="n">
-        <v>2.224273281242684</v>
+        <v>1.920415546901509</v>
       </c>
       <c r="D8" t="n">
-        <v>31.606575</v>
+        <v>9.602077734507544</v>
       </c>
       <c r="E8" t="n">
-        <v>0.457</v>
+        <v>3.126238794575282</v>
       </c>
       <c r="F8" t="n">
-        <v>10.39</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1', '4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-2)', 'Gal(b1-4)', 'GlcNAc(b1-2)']</t>
-        </is>
+        <v>14.14551714285714</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.4429999999999999</v>
+      </c>
+      <c r="H8" t="n">
+        <v>9.254000000000001</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -782,40 +834,46 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Gal(b1-4)GlcNAc(b1-2)Man(a1-3)[Gal(b1-4)GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)[Fuc(a1-6)]GlcNAc</t>
+          <t>Gal(b1-4)GlcNAc(b1-2)Man(a1-6)[GlcNAc(b1-2)Man(a1-3)]Man(b1-4)GlcNAc(b1-4)[Fuc(a1-6)]GlcNAc</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.3559655680542978</v>
+        <v>2.015073259440902</v>
       </c>
       <c r="C9" t="n">
-        <v>2.19766197407428</v>
+        <v>1.721153950190121</v>
       </c>
       <c r="D9" t="n">
-        <v>18.7132125</v>
+        <v>8.605769750950603</v>
       </c>
       <c r="E9" t="n">
-        <v>0.441</v>
+        <v>2.833053165178001</v>
       </c>
       <c r="F9" t="n">
-        <v>7.955</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1', '4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-2)', 'Gal(b1-4)', 'GlcNAc(b1-2)']</t>
-        </is>
+        <v>14.11621333333333</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.4304</v>
+      </c>
+      <c r="H9" t="n">
+        <v>6.459999999999999</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -824,40 +882,46 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Gal(b1-4)GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
+          <t>Gal(b1-4)GlcNAc(b1-2)Man(a1-6)[GlcNAc(b1-2)Man(a1-3)][GlcNAc(b1-4)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.027767814656359</v>
+        <v>0.0696781173686896</v>
       </c>
       <c r="C10" t="n">
-        <v>2.476045733589508</v>
+        <v>1.717471154894835</v>
       </c>
       <c r="D10" t="n">
-        <v>16.46180618061806</v>
+        <v>8.587355774474174</v>
       </c>
       <c r="E10" t="n">
-        <v>0.4375</v>
+        <v>2.800341507190769</v>
       </c>
       <c r="F10" t="n">
-        <v>7.33</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-2)']</t>
-        </is>
+        <v>9.289145714285716</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.453</v>
+      </c>
+      <c r="H10" t="n">
+        <v>7.395999999999999</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -866,40 +930,46 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Gal(b1-4)GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)[Fuc(a1-6)]GlcNAc</t>
+          <t>Gal(b1-4)GlcNAc(b1-2)[Gal(b1-4)GlcNAc(b1-4)]Man(a1-3)[Gal(b1-4)GlcNAc(b1-2)[Gal(b1-4)GlcNAc(b1-6)]Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.142698756269506</v>
+        <v>-0.3833950292321835</v>
       </c>
       <c r="C11" t="n">
-        <v>2.575385896130309</v>
+        <v>1.424187023700174</v>
       </c>
       <c r="D11" t="n">
-        <v>12.52361430523614</v>
+        <v>7.12093511850087</v>
       </c>
       <c r="E11" t="n">
-        <v>0.42</v>
+        <v>2.280139994516561</v>
       </c>
       <c r="F11" t="n">
-        <v>7.595000000000001</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-2)']</t>
-        </is>
+        <v>28.73692571428571</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.4452</v>
+      </c>
+      <c r="H11" t="n">
+        <v>8.001999999999999</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -908,40 +978,46 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Gal(b1-4)GlcNAc(b1-2)Man(a1-6)[GlcNAc(b1-2)Man(a1-3)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
+          <t>Gal(b1-4)GlcNAc(b1-2)[Gal(b1-4)GlcNAc(b1-4)]Man(a1-3)[Gal(b1-4)GlcNAc(b1-2)[Gal(b1-4)GlcNAc(b1-6)]Man(a1-6)]Man(b1-4)GlcNAc(b1-4)[Fuc(a1-6)]GlcNAc</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2.392576267477931</v>
+        <v>-0.4973653096927174</v>
       </c>
       <c r="C12" t="n">
-        <v>2.047297700897916</v>
+        <v>1.371075562924187</v>
       </c>
       <c r="D12" t="n">
-        <v>27.53785714285714</v>
+        <v>6.855377814620937</v>
       </c>
       <c r="E12" t="n">
-        <v>0.479</v>
+        <v>2.466267269448656</v>
       </c>
       <c r="F12" t="n">
-        <v>14.95</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-2)']</t>
-        </is>
+        <v>20.17614666666666</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.4626</v>
+      </c>
+      <c r="H12" t="n">
+        <v>6.428</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -950,40 +1026,46 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Gal(b1-4)GlcNAc(b1-2)Man(a1-6)[GlcNAc(b1-2)Man(a1-3)]Man(b1-4)GlcNAc(b1-4)[Fuc(a1-6)]GlcNAc</t>
+          <t>Gal(b1-4)GlcNAc(b1-2)[GlcNAc(b1-4)]Man(a1-3)[Gal(b1-4)GlcNAc(b1-2)[GlcNAc(b1-6)]Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2.015073259440902</v>
+        <v>-0.4973653096927174</v>
       </c>
       <c r="C13" t="n">
-        <v>1.90563373219762</v>
+        <v>1.325051676537308</v>
       </c>
       <c r="D13" t="n">
-        <v>18.58628333333333</v>
+        <v>6.625258382686541</v>
       </c>
       <c r="E13" t="n">
-        <v>0.473</v>
+        <v>2.04197888509217</v>
       </c>
       <c r="F13" t="n">
-        <v>8.470000000000001</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-2)']</t>
-        </is>
+        <v>16.59388938893889</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.4428</v>
+      </c>
+      <c r="H13" t="n">
+        <v>10.402</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -992,40 +1074,46 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Gal(b1-4)GlcNAc(b1-2)Man(a1-6)[GlcNAc(b1-2)Man(a1-3)][GlcNAc(b1-4)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
+          <t>GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0696781173686896</v>
+        <v>5.003114910265781</v>
       </c>
       <c r="C14" t="n">
-        <v>2.235129157743496</v>
+        <v>2.046759738062542</v>
       </c>
       <c r="D14" t="n">
-        <v>16.40596428571428</v>
+        <v>10.23379869031271</v>
       </c>
       <c r="E14" t="n">
-        <v>0.404</v>
+        <v>3.138514975631664</v>
       </c>
       <c r="F14" t="n">
-        <v>13.735</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-2)']</t>
-        </is>
+        <v>8.928879554622128</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.4360000000000001</v>
+      </c>
+      <c r="H14" t="n">
+        <v>8.048</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -1034,40 +1122,46 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Gal(b1-4)GlcNAc(b1-2)[Gal(b1-4)GlcNAc(b1-4)]Man(a1-3)[Gal(b1-4)GlcNAc(b1-2)[Gal(b1-4)GlcNAc(b1-6)]Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
+          <t>GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)[Fuc(a1-6)]GlcNAc</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.3833950292321835</v>
+        <v>2.637268278006694</v>
       </c>
       <c r="C15" t="n">
-        <v>2.244920453422627</v>
+        <v>2.126228197811836</v>
       </c>
       <c r="D15" t="n">
-        <v>44.48635178571428</v>
+        <v>10.63114098905918</v>
       </c>
       <c r="E15" t="n">
-        <v>0.42025</v>
+        <v>3.183609109940719</v>
       </c>
       <c r="F15" t="n">
-        <v>8.52375</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1', '4C1', '4C1', '4C1', '4C1', '4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-2)', 'Gal(b1-4)', 'GlcNAc(b1-4)', 'Gal(b1-4)', 'GlcNAc(b1-2)', 'Gal(b1-4)', 'GlcNAc(b1-6)']</t>
-        </is>
+        <v>11.004099590041</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.4342</v>
+      </c>
+      <c r="H15" t="n">
+        <v>6.906000000000001</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -1076,40 +1170,46 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Gal(b1-4)GlcNAc(b1-2)[Gal(b1-4)GlcNAc(b1-4)]Man(a1-3)[Gal(b1-4)GlcNAc(b1-2)[Gal(b1-4)GlcNAc(b1-6)]Man(a1-6)]Man(b1-4)GlcNAc(b1-4)[Fuc(a1-6)]GlcNAc</t>
+          <t>GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)][GlcNAc(b1-4)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.4973653096927174</v>
+        <v>1.177593736396362</v>
       </c>
       <c r="C16" t="n">
-        <v>2.194040328027896</v>
+        <v>1.873454516767203</v>
       </c>
       <c r="D16" t="n">
-        <v>33.14937916666667</v>
+        <v>9.367272583836014</v>
       </c>
       <c r="E16" t="n">
-        <v>0.4545</v>
+        <v>2.978851914555812</v>
       </c>
       <c r="F16" t="n">
-        <v>7.45125</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1', '4C1', '4C1', '4C1', '4C1', '4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-2)', 'Gal(b1-4)', 'GlcNAc(b1-4)', 'Gal(b1-4)', 'GlcNAc(b1-2)', 'Gal(b1-4)', 'GlcNAc(b1-6)']</t>
-        </is>
+        <v>11.95979</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.4458</v>
+      </c>
+      <c r="H16" t="n">
+        <v>4.926</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -1118,40 +1218,46 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Gal(b1-4)GlcNAc(b1-2)[GlcNAc(b1-4)]Man(a1-3)[Gal(b1-4)GlcNAc(b1-2)[GlcNAc(b1-6)]Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
+          <t>GlcNAc(b1-2)[GlcNAc(b1-4)]Man(a1-3)[GlcNAc(b1-2)[GlcNAc(b1-6)]Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>-0.4973653096927174</v>
       </c>
       <c r="C17" t="n">
-        <v>1.984343737528825</v>
+        <v>1.760385131113416</v>
       </c>
       <c r="D17" t="n">
-        <v>27.29072907290729</v>
+        <v>8.801925655567082</v>
       </c>
       <c r="E17" t="n">
-        <v>0.4215</v>
+        <v>3.235564404001599</v>
       </c>
       <c r="F17" t="n">
-        <v>11.85</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1', '4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-2)', 'Gal(b1-4)', 'GlcNAc(b1-2)']</t>
-        </is>
+        <v>13.47270666666667</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.4596</v>
+      </c>
+      <c r="H17" t="n">
+        <v>4.978</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -1160,208 +1266,334 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Gal(b1-4)GlcNAc(b1-3)Gal(b1-4)Glc</t>
+          <t>Neu5Ac(a2-3)Gal(b1-4)GlcNAc(b1-2)Man(a1-3)[Neu5Ac(a2-3)Gal(b1-4)GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.1943734671368354</v>
+        <v>-0.2521355456841693</v>
       </c>
       <c r="C18" t="n">
-        <v>2.669142786290044</v>
+        <v>1.752730246278978</v>
       </c>
       <c r="D18" t="n">
-        <v>1.817538246175381</v>
+        <v>8.763651231394888</v>
       </c>
       <c r="E18" t="n">
-        <v>0.4565</v>
+        <v>2.425021331076254</v>
       </c>
       <c r="F18" t="n">
-        <v>3.925</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-3)']</t>
-        </is>
+        <v>22.814132</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.4464</v>
+      </c>
+      <c r="H18" t="n">
+        <v>6.14</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>lipid/free</t>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Gal(b1-4)GlcNAc(b1-3)Gal(b1-4)GlcNAc</t>
+          <t>Neu5Ac(a2-3)Gal(b1-4)GlcNAc(b1-2)Man(a1-3)[Neu5Ac(a2-3)Gal(b1-4)GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)[Fuc(a1-6)]GlcNAc</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.2352308219605394</v>
+        <v>-0.3846626178601627</v>
       </c>
       <c r="C19" t="n">
-        <v>2.63639127321597</v>
+        <v>1.806666759288413</v>
       </c>
       <c r="D19" t="n">
-        <v>4.35031503150315</v>
+        <v>9.033333796442065</v>
       </c>
       <c r="E19" t="n">
-        <v>0.415</v>
+        <v>2.509032411121987</v>
       </c>
       <c r="F19" t="n">
-        <v>6.54</v>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-3)']</t>
-        </is>
+        <v>20.74301236543013</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.4222</v>
+      </c>
+      <c r="H19" t="n">
+        <v>7.837999999999999</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Gal(b1-4)GlcNAc(b1-3)Gal(b1-4)GlcNAc(b1-3)Gal(b1-4)GlcNAc</t>
+          <t>Neu5Ac(a2-3)Gal(b1-4)GlcNAc(b1-2)Man(a1-3)[Neu5Ac(a2-6)Gal(b1-4)GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.2524695696959809</v>
+        <v>-0.2705645907498878</v>
       </c>
       <c r="C20" t="n">
-        <v>2.626073631843238</v>
+        <v>1.676631069036648</v>
       </c>
       <c r="D20" t="n">
-        <v>5.137133333333335</v>
+        <v>8.383155345183241</v>
       </c>
       <c r="E20" t="n">
-        <v>0.4355</v>
+        <v>2.005643627344604</v>
       </c>
       <c r="F20" t="n">
-        <v>9.370000000000001</v>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-3)']</t>
-        </is>
+        <v>18.78958562522919</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.4628</v>
+      </c>
+      <c r="H20" t="n">
+        <v>6.504</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Gal(b1-4)GlcNAc(b1-6)[Gal(b1-3)]GalNAc</t>
+          <t>Neu5Ac(a2-3)Gal(b1-4)GlcNAc(b1-2)Man(a1-6)[Gal(b1-4)GlcNAc(b1-2)Man(a1-3)]Man(b1-4)GlcNAc(b1-4)[Fuc(a1-6)]GlcNAc</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.9947585093047654</v>
+        <v>-0.4973653096927174</v>
       </c>
       <c r="C21" t="n">
-        <v>2.3684476110844</v>
+        <v>1.659696733842132</v>
       </c>
       <c r="D21" t="n">
-        <v>3.6741</v>
+        <v>8.298483669210661</v>
       </c>
       <c r="E21" t="n">
-        <v>0.453</v>
+        <v>2.434442883761228</v>
       </c>
       <c r="F21" t="n">
-        <v>4.105</v>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-6)']</t>
-        </is>
+        <v>18.06837</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.4324</v>
+      </c>
+      <c r="H21" t="n">
+        <v>5.625999999999999</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Neu5Ac(a2-3)Gal(b1-4)GlcNAc(b1-2)Man(a1-6)[Gal(b1-4)GlcNAc(b1-2)Man(a1-3)]Man(b1-4)GlcNAc(b1-4)[Fuc(a1-6)]GlcNAc</t>
+          <t>Neu5Ac(a2-6)Gal(b1-4)GlcNAc(b1-2)Man(a1-3)[Neu5Ac(a2-3)Gal(b1-4)GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.4973653096927174</v>
+        <v>-0.3766844761785684</v>
       </c>
       <c r="C22" t="n">
-        <v>2.532133598783071</v>
+        <v>1.711494808348585</v>
       </c>
       <c r="D22" t="n">
-        <v>22.83945</v>
+        <v>8.557474041742925</v>
       </c>
       <c r="E22" t="n">
-        <v>0.4245</v>
+        <v>2.116459435469261</v>
       </c>
       <c r="F22" t="n">
-        <v>12.695</v>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>['4C1', '4C1']</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>['Gal(b1-4)', 'GlcNAc(b1-2)']</t>
-        </is>
+        <v>24.878828</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.434</v>
+      </c>
+      <c r="H22" t="n">
+        <v>7.303999999999999</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>['Gal(b1-4)GlcNAc']</t>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Neu5Ac(a2-6)Gal(b1-4)GlcNAc(b1-2)Man(a1-3)[Neu5Ac(a2-6)Gal(b1-4)GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)GlcNAc</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>-0.3540072395789538</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1.600404828953631</v>
+      </c>
+      <c r="D23" t="n">
+        <v>8.002024144768157</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2.100542809820641</v>
+      </c>
+      <c r="F23" t="n">
+        <v>22.99092</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.4296</v>
+      </c>
+      <c r="H23" t="n">
+        <v>9.614000000000001</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Neu5Ac(a2-6)Gal(b1-4)GlcNAc(b1-2)Man(a1-3)[Neu5Ac(a2-6)Gal(b1-4)GlcNAc(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)[Fuc(a1-6)]GlcNAc</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>-0.2774388894803677</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1.55570148436109</v>
+      </c>
+      <c r="D24" t="n">
+        <v>7.778507421805449</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1.994761172264495</v>
+      </c>
+      <c r="F24" t="n">
+        <v>22.44650500000001</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.4646</v>
+      </c>
+      <c r="H24" t="n">
+        <v>8.373999999999999</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>['4C1', '4C1', '4C1', '4C1', '4C1']</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)', 'Man(a1-3)', 'Man(b1-4)', 'Man(a1-6)', 'GlcNAc(b1-2)']</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>['GlcNAc(b1-2)Man(a1-3)[GlcNAc(b1-2)Man(a1-6)]Man']</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
         <is>
           <t>N</t>
         </is>

</xml_diff>